<commit_message>
Creating and setting the processes that will scrap all the price info
</commit_message>
<xml_diff>
--- a/Data/Input/InternetPriceMonitoring_Template.xlsx
+++ b/Data/Input/InternetPriceMonitoring_Template.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\UiPath\Dermalogica_Project\Data\Input\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C21F6DF-EDA9-4A26-8D96-863F41BAF58F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,9 +24,77 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>Oz</t>
+  </si>
+  <si>
+    <t>ml</t>
+  </si>
+  <si>
+    <t>Active Moist</t>
+  </si>
+  <si>
+    <t>Age Reversal Eye Complex</t>
+  </si>
+  <si>
+    <t>Calm Water Gel</t>
+  </si>
+  <si>
+    <t>Daily Microfoliant</t>
+  </si>
+  <si>
+    <t>Daily Superfoliant</t>
+  </si>
+  <si>
+    <t>Dynamic Skin Recovery SPF50</t>
+  </si>
+  <si>
+    <t>Intensive Moisture Balance</t>
+  </si>
+  <si>
+    <t>Multi-Active Toner</t>
+  </si>
+  <si>
+    <t>MultiVitamin Power Firm</t>
+  </si>
+  <si>
+    <t>MultiVitamin Power Recovery Masque</t>
+  </si>
+  <si>
+    <t>PreCleanse</t>
+  </si>
+  <si>
+    <t>PreCleanse Balm</t>
+  </si>
+  <si>
+    <t>Skin Hydrating Masque</t>
+  </si>
+  <si>
+    <t>Skin Smoothing Cream</t>
+  </si>
+  <si>
+    <t>Sound Sleep Cocoon</t>
+  </si>
+  <si>
+    <t>Special Cleansing Gel</t>
+  </si>
+  <si>
+    <t>Stress Positive Eye Lift</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -28,16 +102,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -45,12 +139,39 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +451,261 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S15" sqref="S15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="4">
+        <v>3.4</v>
+      </c>
+      <c r="C2" s="4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="4">
+        <v>1.7</v>
+      </c>
+      <c r="C3" s="4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="C4" s="4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="4">
+        <v>1.7</v>
+      </c>
+      <c r="C5" s="4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="4">
+        <v>2.6</v>
+      </c>
+      <c r="C6" s="4">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="4">
+        <v>2</v>
+      </c>
+      <c r="C7" s="4">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="4">
+        <v>1.7</v>
+      </c>
+      <c r="C8" s="4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="4">
+        <v>3.4</v>
+      </c>
+      <c r="C9" s="4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4">
+        <v>1.7</v>
+      </c>
+      <c r="C10" s="4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4">
+        <v>8.4</v>
+      </c>
+      <c r="C11" s="4">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="C12" s="4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="C13" s="4">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="4">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="C14" s="4">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="4">
+        <v>3</v>
+      </c>
+      <c r="C15" s="4">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="C16" s="4">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="4">
+        <v>3.4</v>
+      </c>
+      <c r="C17" s="4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="4">
+        <v>1.7</v>
+      </c>
+      <c r="C18" s="4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="4">
+        <v>1.7</v>
+      </c>
+      <c r="C19" s="4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="4">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="C20" s="4">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="4">
+        <v>8.4</v>
+      </c>
+      <c r="C21" s="4">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="4">
+        <v>0.85</v>
+      </c>
+      <c r="C22" s="4">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixing errors on extracting the prices for USA page
</commit_message>
<xml_diff>
--- a/Data/Input/InternetPriceMonitoring_Template.xlsx
+++ b/Data/Input/InternetPriceMonitoring_Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\UiPath\Dermalogica_Project\Data\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C21F6DF-EDA9-4A26-8D96-863F41BAF58F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6600717B-BBD0-4224-A0CE-29F74B0B0526}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -91,8 +91,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -158,7 +159,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -170,6 +171,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -455,7 +459,7 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S15" sqref="S15"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -533,7 +537,7 @@
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="5">
         <v>2</v>
       </c>
       <c r="C7" s="4">
@@ -621,7 +625,7 @@
       <c r="A15" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B15" s="5">
         <v>3</v>
       </c>
       <c r="C15" s="4">

</xml_diff>

<commit_message>
First steps on UK website process
</commit_message>
<xml_diff>
--- a/Data/Input/InternetPriceMonitoring_Template.xlsx
+++ b/Data/Input/InternetPriceMonitoring_Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\UiPath\Dermalogica_Project\Data\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6600717B-BBD0-4224-A0CE-29F74B0B0526}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A05BA60-F893-48D0-B6B8-39858E82D64A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -91,9 +91,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
-    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -173,7 +172,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -459,7 +458,7 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>